<commit_message>
Fix abs ref issue and add cumulative time
</commit_message>
<xml_diff>
--- a/Time Accounting/Time Accounting.xlsx
+++ b/Time Accounting/Time Accounting.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Billable Amount</t>
+  </si>
+  <si>
+    <t>Productive</t>
+  </si>
+  <si>
+    <t>Cumulative Productive Minutes</t>
   </si>
 </sst>
 </file>
@@ -145,13 +151,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -454,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H343"/>
+  <dimension ref="A1:J343"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,12 +476,14 @@
     <col min="3" max="3" width="8.28515625" customWidth="1"/>
     <col min="4" max="4" width="62.85546875" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,16 +500,22 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>41233</v>
       </c>
@@ -509,21 +526,28 @@
         <v>0.34027777777777773</v>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
-        <f>ROUND((C2-B2)*24*60,1)</f>
-        <v>10</v>
-      </c>
-      <c r="H2" s="5">
-        <f>IF(E2,G2*(Configuration!B3/60),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f t="shared" ref="H2:H38" si="0">ROUND((C2-B2)*24*60,1)</f>
+        <v>10</v>
+      </c>
+      <c r="I2" s="5">
+        <f>IF(E2,H2*(Configuration!$B$3/60),0)</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="J2">
+        <f>IF(F2,H2,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>A2</f>
         <v>41233</v>
@@ -533,690 +557,834 @@
         <v>0.34027777777777773</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="G3">
-        <f>ROUND((C3-B3)*24*60,1)</f>
+      <c r="H3">
+        <f t="shared" si="0"/>
         <v>-490</v>
       </c>
-      <c r="H3" s="5">
-        <f>G3*(Configuration!B4/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="5">
+        <f>IF(E3,H3*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f>J2+IF(F3,H3,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A38" si="0">A3</f>
+        <f t="shared" ref="A4:A38" si="1">A3</f>
         <v>41233</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B38" si="1">C3</f>
+        <f t="shared" ref="B4:B38" si="2">C3</f>
         <v>0</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="G4">
-        <f>ROUND((C4-B4)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <f>G4*(Configuration!B5/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <f>IF(E4,H4*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J38" si="3">J3+IF(F4,H4,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="G5">
-        <f>ROUND((C5-B5)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
-        <f>G5*(Configuration!B6/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <f>IF(E5,H5*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="G6">
-        <f>ROUND((C6-B6)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <f>G6*(Configuration!B7/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <f>IF(E6,H6*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="G7">
-        <f>ROUND((C7-B7)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <f>G7*(Configuration!B8/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <f>IF(E7,H7*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="G8">
-        <f>ROUND((C8-B8)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <f>G8*(Configuration!B9/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <f>IF(E8,H8*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="G9">
-        <f>ROUND((C9-B9)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <f>G9*(Configuration!B10/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <f>IF(E9,H9*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="G10">
-        <f>ROUND((C10-B10)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
-        <f>G10*(Configuration!B11/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <f>IF(E10,H10*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="G11">
-        <f>ROUND((C11-B11)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
-        <f>G11*(Configuration!B12/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <f>IF(E11,H11*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B12" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <f>ROUND((C12-B12)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="5">
-        <f>G12*(Configuration!B13/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <f>IF(E12,H12*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <f>ROUND((C13-B13)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="5">
-        <f>G13*(Configuration!B14/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <f>IF(E13,H13*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B14" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <f>ROUND((C14-B14)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="5">
-        <f>G14*(Configuration!B15/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <f>IF(E14,H14*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <f>ROUND((C15-B15)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="5">
-        <f>G15*(Configuration!B16/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <f>IF(E15,H15*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B16" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <f>ROUND((C16-B16)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="5">
-        <f>G16*(Configuration!B17/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <f>IF(E16,H16*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <f>ROUND((C17-B17)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="5">
-        <f>G17*(Configuration!B18/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <f>IF(E17,H17*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B18" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <f>ROUND((C18-B18)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <f>G18*(Configuration!B19/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <f>IF(E18,H18*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <f>ROUND((C19-B19)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="5">
-        <f>G19*(Configuration!B20/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <f>IF(E19,H19*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B20" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <f>ROUND((C20-B20)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="5">
-        <f>G20*(Configuration!B21/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <f>IF(E20,H20*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B21" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <f>ROUND((C21-B21)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
-        <f>G21*(Configuration!B22/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <f>IF(E21,H21*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B22" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <f>ROUND((C22-B22)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="5">
-        <f>G22*(Configuration!B23/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <f>IF(E22,H22*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B23" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <f>ROUND((C23-B23)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="5">
-        <f>G23*(Configuration!B24/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <f>IF(E23,H23*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B24" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <f>ROUND((C24-B24)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="5">
-        <f>G24*(Configuration!B25/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <f>IF(E24,H24*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B25" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <f>ROUND((C25-B25)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="5">
-        <f>G25*(Configuration!B26/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
+        <f>IF(E25,H25*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <f>ROUND((C26-B26)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="5">
-        <f>G26*(Configuration!B27/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
+        <f>IF(E26,H26*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B27" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <f>ROUND((C27-B27)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="5">
-        <f>G27*(Configuration!B28/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
+        <f>IF(E27,H27*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B28" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <f>ROUND((C28-B28)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="5">
-        <f>G28*(Configuration!B29/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="5">
+        <f>IF(E28,H28*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B29" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <f>ROUND((C29-B29)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="5">
-        <f>G29*(Configuration!B30/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <f>IF(E29,H29*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B30" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <f>ROUND((C30-B30)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="5">
-        <f>G30*(Configuration!B31/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <f>IF(E30,H30*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <f>ROUND((C31-B31)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="5">
-        <f>G31*(Configuration!B32/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <f>IF(E31,H31*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B32" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <f>ROUND((C32-B32)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="5">
-        <f>G32*(Configuration!B33/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <f>IF(E32,H32*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <f>ROUND((C33-B33)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="5">
-        <f>G33*(Configuration!B34/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <f>IF(E33,H33*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B34" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <f>ROUND((C34-B34)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="5">
-        <f>G34*(Configuration!B35/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="5">
+        <f>IF(E34,H34*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B35" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <f>ROUND((C35-B35)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="5">
-        <f>G35*(Configuration!B36/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <f>IF(E35,H35*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <f>ROUND((C36-B36)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="5">
-        <f>G36*(Configuration!B37/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="5">
+        <f>IF(E36,H36*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B37" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <f>ROUND((C37-B37)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="5">
-        <f>G37*(Configuration!B38/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
+        <f>IF(E37,H37*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41233</v>
       </c>
       <c r="B38" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <f>ROUND((C38-B38)*24*60,1)</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="5">
-        <f>G38*(Configuration!B39/60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="5">
+        <f>IF(E38,H38*(Configuration!$B$3/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
     </row>
@@ -2402,7 +2570,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576"/>
+    <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2412,7 +2580,7 @@
           <x14:formula1>
             <xm:f>'Billable Entities'!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F1048576</xm:sqref>
+          <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>